<commit_message>
minor changes to file links
</commit_message>
<xml_diff>
--- a/src/dams_mcda/www/DecisionMatrices_updated.xlsx
+++ b/src/dams_mcda/www/DecisionMatrices_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emma\Documents\R_ELF\R_NEST\MCDA_App_Shiny\MCDA_11042019\src\dams_mcda\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0948AB-AB12-47E7-A9FD-AB41D89416AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3DE4C2-F1FA-4B2C-B531-B1B0C9324334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="396" windowWidth="17280" windowHeight="8964" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="10" r:id="rId1"/>
@@ -448,9 +448,6 @@
     <t>Aesthetic Value †</t>
   </si>
   <si>
-    <t xml:space="preserve">*1 GW = 1000 MW, so to convert from GW to MW, multiply the value by 1,000. To convert from MW to GW, divide by 1,000. °Indigenous cultural traditions and lifeways data come from a survey of a sample of Penobscot Nation citizens (N=2), supported by researcher observations of informal conversations with Penobscot Nation citizens and representatives. †Cells are blank because we do not have data for these decision criteria. </t>
-  </si>
-  <si>
     <t>Adjusted for inflation using: https://www.calculator.net/inflation-calculator.html?cstartingamount1=1&amp;cinyear1=2014&amp;coutyear1=2019&amp;calctype=1&amp;x=124&amp;y=20</t>
   </si>
   <si>
@@ -578,6 +575,9 @@
   </si>
   <si>
     <t>B. Blachly and E. Uchida, Estimating the Marginal Cost of Dam Removal, in Environmental and Natural Resource Economics Working Papers, 2017, vol. Paper 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*1 GW = 1000 MW, so to convert from GW to MW, multiply the value by 1,000. To convert from MW to GW, divide by 1,000. °Indigenous cultural traditions and lifeways data come from a survey of a sample of Penobscot Nation citizens (N=2), supported by researcher observations of informal conversations with Penobscot Nation citizens and representatives. †Cells are zero because we do not have data for these decision criteria. </t>
   </si>
 </sst>
 </file>
@@ -1043,9 +1043,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1057,6 +1054,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1710,7 +1710,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1725,7 +1725,7 @@
     </row>
     <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="75"/>
       <c r="C5" s="75"/>
@@ -1735,17 +1735,17 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="75" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1758,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2068,14 +2068,14 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
+      <c r="A14" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="51"/>
@@ -5021,7 +5021,7 @@
   </sheetPr>
   <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G19" sqref="G19"/>
     </sheetView>
@@ -5033,7 +5033,7 @@
     <col min="3" max="3" width="12.44140625" style="11" customWidth="1"/>
     <col min="4" max="4" width="48.77734375" style="11" customWidth="1"/>
     <col min="5" max="5" width="49" style="11" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="79"/>
+    <col min="6" max="6" width="14.44140625" style="78"/>
     <col min="8" max="8" width="47.6640625" style="11" customWidth="1"/>
     <col min="9" max="16384" width="14.44140625" style="11"/>
   </cols>
@@ -5084,7 +5084,7 @@
     </row>
     <row r="2" spans="1:26" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>96</v>
@@ -5094,7 +5094,7 @@
       </c>
       <c r="D2"/>
       <c r="E2" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>14</v>
@@ -5178,7 +5178,7 @@
       </c>
       <c r="D4"/>
       <c r="E4" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>14</v>
@@ -5213,7 +5213,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>93</v>
@@ -5224,14 +5224,14 @@
       <c r="E5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="78" t="s">
-        <v>156</v>
+      <c r="F5" s="77" t="s">
+        <v>155</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -5257,7 +5257,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>93</v>
@@ -5266,16 +5266,16 @@
         <v>34</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="77" t="s">
-        <v>156</v>
+      <c r="G6" s="76" t="s">
+        <v>155</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -5301,25 +5301,25 @@
         <v>36</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F7" s="78" t="s">
-        <v>156</v>
+        <v>142</v>
+      </c>
+      <c r="F7" s="77" t="s">
+        <v>155</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>37</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -5345,25 +5345,25 @@
         <v>38</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>141</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="77" t="s">
-        <v>156</v>
+      <c r="G8" s="76" t="s">
+        <v>155</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -5389,7 +5389,7 @@
         <v>39</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>93</v>
@@ -5407,7 +5407,7 @@
         <v>18</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -5526,7 +5526,7 @@
         <v>18</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F12" s="36" t="s">
         <v>48</v>
@@ -5565,10 +5565,10 @@
         <v>93</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E13" s="60" t="s">
         <v>151</v>
-      </c>
-      <c r="E13" s="60" t="s">
-        <v>152</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>50</v>
@@ -5612,7 +5612,7 @@
         <v>18</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>52</v>
@@ -5688,7 +5688,7 @@
     </row>
     <row r="16" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>43</v>
@@ -5700,7 +5700,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>52</v>
@@ -5823,22 +5823,22 @@
         <v>60</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C19" s="34" t="s">
         <v>94</v>
       </c>
       <c r="D19" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="40" t="s">
         <v>132</v>
-      </c>
-      <c r="E19" s="40" t="s">
-        <v>133</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="81" t="s">
-        <v>157</v>
+      <c r="G19" s="80" t="s">
+        <v>156</v>
       </c>
       <c r="H19" s="41" t="s">
         <v>100</v>
@@ -5867,7 +5867,7 @@
         <v>61</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>94</v>
@@ -5911,7 +5911,7 @@
         <v>64</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>94</v>
@@ -5955,7 +5955,7 @@
         <v>67</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>94</v>
@@ -5999,7 +5999,7 @@
         <v>70</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>94</v>
@@ -6010,8 +6010,8 @@
       <c r="E23" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="80" t="s">
-        <v>156</v>
+      <c r="F23" s="79" t="s">
+        <v>155</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>73</v>
@@ -33632,9 +33632,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2:F13"/>
+      <selection pane="topRight" activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -33943,14 +33943,14 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
+      <c r="A14" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -34941,8 +34941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F13"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -35251,14 +35251,14 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
+      <c r="A14" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="51"/>
@@ -38201,8 +38201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F13"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -38507,14 +38507,14 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
+      <c r="A14" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="51"/>
@@ -41457,8 +41457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F13"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -41767,14 +41767,14 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
+      <c r="A14" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="51"/>
@@ -44717,8 +44717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F13"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -45027,14 +45027,14 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
+      <c r="A14" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="51"/>
@@ -47977,8 +47977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A13" sqref="A2:A13"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -48287,14 +48287,14 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
+      <c r="A14" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="51"/>
@@ -51238,8 +51238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F13"/>
+    <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -51548,14 +51548,14 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
+      <c r="A14" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="51"/>

</xml_diff>